<commit_message>
Update Arbeidsmarkedstilknytting for Vestfold i 2022 SSB 13563.xlsx
Oppdateringer
</commit_message>
<xml_diff>
--- a/03_Arbeid og næringsliv/Sysselsetting/2022/Arbeidsmarkedstilknytting for Vestfold i 2022 SSB 13563.xlsx
+++ b/03_Arbeid og næringsliv/Sysselsetting/2022/Arbeidsmarkedstilknytting for Vestfold i 2022 SSB 13563.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/ellen_just_hansen_vestfoldfylke_no/Documents/Dokumenter/GitHub/Github-Kunnskap-om-Vestfold/Vestfold/03_Arbeid og næringsliv/Sysselsetting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/ellen_just_hansen_vestfoldfylke_no/Documents/Dokumenter/GitHub/Nyeste Github versjon/Vestfold/03_Arbeid og næringsliv/Sysselsetting/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{305BF331-A212-4E48-AEE8-C4B1389B4381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="1080" windowWidth="23145" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosatte" sheetId="2" r:id="rId1"/>
@@ -453,20 +453,20 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -492,7 +492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -521,7 +521,7 @@
         <v>210443</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -550,7 +550,7 @@
         <v>9557</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -579,7 +579,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -608,7 +608,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -637,7 +637,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -666,7 +666,7 @@
         <v>2723</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -695,7 +695,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -724,7 +724,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -733,7 +733,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -742,7 +742,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
@@ -766,7 +766,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -800,7 +800,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -834,7 +834,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -868,7 +868,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -902,7 +902,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -936,7 +936,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -970,7 +970,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1047,7 +1047,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1056,7 +1056,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1065,7 +1065,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1074,7 +1074,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1083,7 +1083,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>

</xml_diff>